<commit_message>
just testpoints and sample report files
</commit_message>
<xml_diff>
--- a/inst/testdata/test_api_output_1mile_testpoints50.xlsx
+++ b/inst/testdata/test_api_output_1mile_testpoints50.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorrale\R\mysource\EJAM\inst\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FF2856-30E9-4AF5-A115-E854DB6DB82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA8673F-1607-4328-BD17-4E48738FBD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="19640" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14040" yWindow="795" windowWidth="14025" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EJ stats" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1081,7 +1094,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1153,10 +1166,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1500,30 +1513,30 @@
   <dimension ref="A1:ES51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY1" sqref="AY1"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.90625" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" customWidth="1"/>
-    <col min="3" max="3" width="6.54296875" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" customWidth="1"/>
-    <col min="5" max="5" width="8.08984375" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="6" customWidth="1"/>
-    <col min="11" max="18" width="6.90625" customWidth="1"/>
-    <col min="19" max="22" width="6.26953125" customWidth="1"/>
+    <col min="11" max="18" width="6.85546875" customWidth="1"/>
+    <col min="19" max="22" width="6.28515625" customWidth="1"/>
     <col min="26" max="40" width="9" customWidth="1"/>
-    <col min="41" max="50" width="7.1796875" customWidth="1"/>
+    <col min="41" max="50" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:149" s="2" customFormat="1" ht="134" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:149" s="2" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1985,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>307</v>
       </c>
@@ -2421,7 +2434,7 @@
         <v>41.067363499999999</v>
       </c>
     </row>
-    <row r="3" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>320</v>
       </c>
@@ -2870,7 +2883,7 @@
         <v>40.7291338</v>
       </c>
     </row>
-    <row r="4" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>161</v>
       </c>
@@ -3319,7 +3332,7 @@
         <v>40.830450800000001</v>
       </c>
     </row>
-    <row r="5" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>236</v>
       </c>
@@ -3768,7 +3781,7 @@
         <v>38.940542200000003</v>
       </c>
     </row>
-    <row r="6" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>212</v>
       </c>
@@ -4217,7 +4230,7 @@
         <v>44.983989200000003</v>
       </c>
     </row>
-    <row r="7" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>348</v>
       </c>
@@ -4651,7 +4664,7 @@
         <v>40.746471499999998</v>
       </c>
     </row>
-    <row r="8" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>272</v>
       </c>
@@ -5085,7 +5098,7 @@
         <v>31.2246509</v>
       </c>
     </row>
-    <row r="9" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>277</v>
       </c>
@@ -5519,7 +5532,7 @@
         <v>25.631220899999999</v>
       </c>
     </row>
-    <row r="10" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>264</v>
       </c>
@@ -5953,7 +5966,7 @@
         <v>27.744837499999999</v>
       </c>
     </row>
-    <row r="11" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>342</v>
       </c>
@@ -6402,7 +6415,7 @@
         <v>36.160001700000002</v>
       </c>
     </row>
-    <row r="12" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>304</v>
       </c>
@@ -6851,7 +6864,7 @@
         <v>32.923276600000001</v>
       </c>
     </row>
-    <row r="13" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>194</v>
       </c>
@@ -7285,7 +7298,7 @@
         <v>40.639372100000003</v>
       </c>
     </row>
-    <row r="14" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>301</v>
       </c>
@@ -7719,7 +7732,7 @@
         <v>30.5113111</v>
       </c>
     </row>
-    <row r="15" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>255</v>
       </c>
@@ -8168,7 +8181,7 @@
         <v>43.180906999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>249</v>
       </c>
@@ -8602,7 +8615,7 @@
         <v>27.424755600000001</v>
       </c>
     </row>
-    <row r="17" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>298</v>
       </c>
@@ -9051,7 +9064,7 @@
         <v>39.129921600000003</v>
       </c>
     </row>
-    <row r="18" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>156</v>
       </c>
@@ -9500,7 +9513,7 @@
         <v>41.061382100000003</v>
       </c>
     </row>
-    <row r="19" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>202</v>
       </c>
@@ -9934,7 +9947,7 @@
         <v>27.9278078</v>
       </c>
     </row>
-    <row r="20" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>323</v>
       </c>
@@ -10353,7 +10366,7 @@
         <v>40.6618201</v>
       </c>
     </row>
-    <row r="21" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>244</v>
       </c>
@@ -10802,7 +10815,7 @@
         <v>38.8064787</v>
       </c>
     </row>
-    <row r="22" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>261</v>
       </c>
@@ -11236,7 +11249,7 @@
         <v>40.759007199999999</v>
       </c>
     </row>
-    <row r="23" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>174</v>
       </c>
@@ -11655,7 +11668,7 @@
         <v>44.9632249</v>
       </c>
     </row>
-    <row r="24" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>285</v>
       </c>
@@ -12104,7 +12117,7 @@
         <v>41.691692799999998</v>
       </c>
     </row>
-    <row r="25" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>179</v>
       </c>
@@ -12553,7 +12566,7 @@
         <v>36.564103899999999</v>
       </c>
     </row>
-    <row r="26" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>258</v>
       </c>
@@ -13002,7 +13015,7 @@
         <v>39.397665099999998</v>
       </c>
     </row>
-    <row r="27" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>233</v>
       </c>
@@ -13436,7 +13449,7 @@
         <v>34.409537299999997</v>
       </c>
     </row>
-    <row r="28" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>267</v>
       </c>
@@ -13885,7 +13898,7 @@
         <v>34.051664899999999</v>
       </c>
     </row>
-    <row r="29" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>295</v>
       </c>
@@ -14334,7 +14347,7 @@
         <v>42.527658099999996</v>
       </c>
     </row>
-    <row r="30" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>339</v>
       </c>
@@ -14783,7 +14796,7 @@
         <v>37.368432599999998</v>
       </c>
     </row>
-    <row r="31" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>207</v>
       </c>
@@ -15217,7 +15230,7 @@
         <v>47.757151700000001</v>
       </c>
     </row>
-    <row r="32" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>217</v>
       </c>
@@ -15651,7 +15664,7 @@
         <v>39.253299200000001</v>
       </c>
     </row>
-    <row r="33" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>315</v>
       </c>
@@ -16085,7 +16098,7 @@
         <v>35.232977099999999</v>
       </c>
     </row>
-    <row r="34" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>345</v>
       </c>
@@ -16534,7 +16547,7 @@
         <v>40.497771800000002</v>
       </c>
     </row>
-    <row r="35" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>184</v>
       </c>
@@ -16983,7 +16996,7 @@
         <v>40.385940099999999</v>
       </c>
     </row>
-    <row r="36" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>312</v>
       </c>
@@ -17417,7 +17430,7 @@
         <v>29.578689300000001</v>
       </c>
     </row>
-    <row r="37" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>336</v>
       </c>
@@ -17866,7 +17879,7 @@
         <v>40.481440399999997</v>
       </c>
     </row>
-    <row r="38" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>239</v>
       </c>
@@ -18315,7 +18328,7 @@
         <v>39.114590800000002</v>
       </c>
     </row>
-    <row r="39" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>333</v>
       </c>
@@ -18764,7 +18777,7 @@
         <v>40.383804599999998</v>
       </c>
     </row>
-    <row r="40" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>225</v>
       </c>
@@ -19213,7 +19226,7 @@
         <v>40.486102199999998</v>
       </c>
     </row>
-    <row r="41" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>290</v>
       </c>
@@ -19662,7 +19675,7 @@
         <v>43.014536200000002</v>
       </c>
     </row>
-    <row r="42" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>280</v>
       </c>
@@ -20111,7 +20124,7 @@
         <v>34.579271400000003</v>
       </c>
     </row>
-    <row r="43" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>149</v>
       </c>
@@ -20560,7 +20573,7 @@
         <v>33.560416199999999</v>
       </c>
     </row>
-    <row r="44" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>252</v>
       </c>
@@ -21009,7 +21022,7 @@
         <v>42.732305099999998</v>
       </c>
     </row>
-    <row r="45" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>230</v>
       </c>
@@ -21443,7 +21456,7 @@
         <v>39.678192199999998</v>
       </c>
     </row>
-    <row r="46" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>328</v>
       </c>
@@ -21892,7 +21905,7 @@
         <v>38.386394500000002</v>
       </c>
     </row>
-    <row r="47" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>197</v>
       </c>
@@ -22341,7 +22354,7 @@
         <v>34.747686199999997</v>
       </c>
     </row>
-    <row r="48" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>222</v>
       </c>
@@ -22775,7 +22788,7 @@
         <v>36.934159299999997</v>
       </c>
     </row>
-    <row r="49" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>189</v>
       </c>
@@ -23209,7 +23222,7 @@
         <v>41.746000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>164</v>
       </c>
@@ -23406,7 +23419,7 @@
         <v>33.601434400000002</v>
       </c>
     </row>
-    <row r="51" spans="1:149" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>169</v>
       </c>

</xml_diff>